<commit_message>
Update to case study and simulation code
</commit_message>
<xml_diff>
--- a/CaseStudy3_Scharf2024/Outputs/Reproduction_Kfold_scenario_2_2AGGx2Resample_SHAPE_UTH_CL_24082025160859/Reproduction_Kfold_scenario_2_2AGGx2Resample_SHAPE_UTH_CL_24082025161537.xlsx
+++ b/CaseStudy3_Scharf2024/Outputs/Reproduction_Kfold_scenario_2_2AGGx2Resample_SHAPE_UTH_CL_24082025160859/Reproduction_Kfold_scenario_2_2AGGx2Resample_SHAPE_UTH_CL_24082025161537.xlsx
@@ -5,18 +5,31 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://curtin-my.sharepoint.com/personal/283284g_curtin_edu_au/Documents/PycharmProjects/HierarchicalDataPaper/CaseStudy3_Scharf2024/Outputs/Results_Kfold_scenario_2_2AGGx2Resample_SHAPE_UTH_CL_24082025160859/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://curtin-my.sharepoint.com/personal/283284g_curtin_edu_au/Documents/PycharmProjects/HierarchicalDataPaper/CaseStudy3_Scharf2024/Outputs/Reproduction_Kfold_scenario_2_2AGGx2Resample_SHAPE_UTH_CL_24082025160859/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{E8D7E67B-8911-400E-9F9D-39EE48AE81F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD4BB5C-C1CB-45FF-BAC8-0F62CB1A00FB}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{E8D7E67B-8911-400E-9F9D-39EE48AE81F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7861F9C9-93DB-4CD7-90B3-DCA70C807E62}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A233C7D3-027F-4630-B902-8A65963FD7CF}"/>
+    <workbookView xWindow="-22860" yWindow="1440" windowWidth="17280" windowHeight="8925" activeTab="1" xr2:uid="{A233C7D3-027F-4630-B902-8A65963FD7CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Kfold_scenario_2_2AGGx2Resample" sheetId="1" r:id="rId1"/>
     <sheet name="Kfold_summary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -621,6 +634,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8234,10 +8251,13 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">

</xml_diff>